<commit_message>
move exams to a separate folder
</commit_message>
<xml_diff>
--- a/08-cost-sharing/shapley.xlsx
+++ b/08-cost-sharing/shapley.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Shapley Not Modular" sheetId="1" state="visible" r:id="rId2"/>
@@ -61,6 +61,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">קבוצה</t>
     </r>
@@ -70,6 +71,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -90,6 +92,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -99,6 +102,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -108,6 +112,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -119,6 +124,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -128,6 +134,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -137,6 +144,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -148,6 +156,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -157,6 +166,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -166,6 +176,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -177,6 +188,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -186,6 +198,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -195,6 +208,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -204,6 +218,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -213,6 +228,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -224,6 +240,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">עלות</t>
     </r>
@@ -233,6 +250,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -244,6 +262,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">סדר</t>
     </r>
@@ -253,6 +272,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -264,6 +284,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -273,6 +294,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -282,6 +304,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -291,6 +314,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -300,6 +324,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -311,6 +336,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -320,6 +346,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -329,6 +356,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -338,6 +366,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -347,6 +376,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -358,6 +388,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -367,6 +398,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -376,6 +408,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -385,6 +418,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -394,6 +428,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -405,6 +440,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -414,6 +450,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -423,6 +460,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -432,6 +470,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -441,6 +480,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -452,6 +492,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -461,6 +502,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -470,6 +512,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -479,6 +522,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -488,6 +532,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -499,6 +544,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -508,6 +554,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -517,6 +564,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -526,6 +574,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -535,6 +584,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -549,6 +599,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">א</t>
     </r>
@@ -558,6 +609,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -569,6 +621,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ב</t>
     </r>
@@ -578,6 +631,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -589,6 +643,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ג</t>
     </r>
@@ -598,6 +653,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -609,6 +665,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">סכום</t>
     </r>
@@ -618,6 +675,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -629,6 +687,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">עלות בלי ג</t>
     </r>
@@ -638,6 +697,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -649,6 +709,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ערך נוסע א</t>
     </r>
@@ -658,6 +719,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -669,6 +731,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ערך נוסע ב</t>
     </r>
@@ -678,6 +741,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -689,6 +753,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ערך נוסע ג</t>
     </r>
@@ -698,6 +763,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -709,6 +775,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ערך </t>
     </r>
@@ -718,6 +785,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"</t>
     </r>
@@ -727,6 +795,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">נהג</t>
     </r>
@@ -736,6 +805,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">":</t>
     </r>
@@ -747,6 +817,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">נבחר</t>
     </r>
@@ -756,6 +827,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -767,6 +839,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">סכום בלי א</t>
     </r>
@@ -776,6 +849,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -787,6 +861,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">סכום בלי ב</t>
     </r>
@@ -796,6 +871,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -807,6 +883,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">סכום בלי ג</t>
     </r>
@@ -816,6 +893,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -836,6 +914,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">נהג</t>
     </r>
@@ -845,6 +924,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -859,6 +939,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">תשלום נוסע א</t>
     </r>
@@ -868,6 +949,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -879,6 +961,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">תשלום נוסע ב</t>
     </r>
@@ -888,6 +971,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -899,6 +983,7 @@
         <sz val="10"/>
         <rFont val="Nachlieli CLM"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">תשלום נוסע ג</t>
     </r>
@@ -908,6 +993,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
@@ -927,6 +1013,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -944,27 +1031,31 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Nachlieli CLM"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="10"/>
       <name val="Nachlieli CLM"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Nachlieli CLM"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Nachlieli CLM"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1050,16 +1141,20 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1136,10 +1231,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1158,10 +1249,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1200,10 +1287,10 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Result" xfId="20"/>
-    <cellStyle name="Result2" xfId="21"/>
-    <cellStyle name="Heading" xfId="22"/>
-    <cellStyle name="Heading1" xfId="23"/>
+    <cellStyle name="Heading 3" xfId="20"/>
+    <cellStyle name="Heading1" xfId="21"/>
+    <cellStyle name="Result" xfId="22"/>
+    <cellStyle name="Result2" xfId="23"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1275,7 +1362,7 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1286,9 +1373,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
@@ -1722,7 +1809,7 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1733,9 +1820,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
@@ -2154,7 +2241,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2169,7 +2256,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2180,9 +2267,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
@@ -2407,7 +2494,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2422,8 +2509,8 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2433,9 +2520,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
@@ -2669,7 +2756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
         <v>26</v>
       </c>
@@ -2706,31 +2793,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="20" t="n">
+      <c r="B12" s="19" t="n">
         <f aca="false">B$9-B4</f>
         <v>0</v>
       </c>
-      <c r="C12" s="20" t="n">
+      <c r="C12" s="19" t="n">
         <f aca="false">C$9-C4</f>
         <v>-10</v>
       </c>
-      <c r="D12" s="20" t="n">
+      <c r="D12" s="19" t="n">
         <f aca="false">D$9-D4</f>
         <v>7</v>
       </c>
-      <c r="E12" s="20" t="n">
+      <c r="E12" s="19" t="n">
         <f aca="false">E$9-E4</f>
         <v>-9</v>
       </c>
-      <c r="F12" s="20" t="n">
+      <c r="F12" s="19" t="n">
         <f aca="false">F$9-F4</f>
         <v>2</v>
       </c>
-      <c r="G12" s="20" t="n">
+      <c r="G12" s="19" t="n">
         <f aca="false">G$9-G4</f>
         <v>-9</v>
       </c>
@@ -2738,12 +2825,12 @@
         <f aca="false">H$9-H4</f>
         <v>8</v>
       </c>
-      <c r="I12" s="20" t="n">
+      <c r="I12" s="19" t="n">
         <f aca="false">I$9-I4</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
@@ -2751,52 +2838,52 @@
         <f aca="false">B$9-B5</f>
         <v>0</v>
       </c>
-      <c r="C13" s="20" t="n">
+      <c r="C13" s="19" t="n">
         <f aca="false">C$9-C5</f>
         <v>-2</v>
       </c>
-      <c r="D13" s="20" t="n">
+      <c r="D13" s="19" t="n">
         <f aca="false">D$9-D5</f>
         <v>-15</v>
       </c>
-      <c r="E13" s="20" t="n">
+      <c r="E13" s="19" t="n">
         <f aca="false">E$9-E5</f>
         <v>-9</v>
       </c>
-      <c r="F13" s="20" t="n">
+      <c r="F13" s="19" t="n">
         <f aca="false">F$9-F5</f>
         <v>-12</v>
       </c>
-      <c r="G13" s="20" t="n">
+      <c r="G13" s="19" t="n">
         <f aca="false">G$9-G5</f>
         <v>-1</v>
       </c>
-      <c r="H13" s="20" t="n">
+      <c r="H13" s="19" t="n">
         <f aca="false">H$9-H5</f>
         <v>-14</v>
       </c>
-      <c r="I13" s="20" t="n">
+      <c r="I13" s="19" t="n">
         <f aca="false">I$9-I5</f>
         <v>-13</v>
       </c>
     </row>
-    <row r="14" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="20" t="n">
+      <c r="B14" s="19" t="n">
         <f aca="false">B$9-B6</f>
         <v>0</v>
       </c>
-      <c r="C14" s="20" t="n">
+      <c r="C14" s="19" t="n">
         <f aca="false">C$9-C6</f>
         <v>-2</v>
       </c>
-      <c r="D14" s="20" t="n">
+      <c r="D14" s="19" t="n">
         <f aca="false">D$9-D6</f>
         <v>7</v>
       </c>
-      <c r="E14" s="20" t="n">
+      <c r="E14" s="19" t="n">
         <f aca="false">E$9-E6</f>
         <v>-25</v>
       </c>
@@ -2804,120 +2891,116 @@
         <f aca="false">F$9-F6</f>
         <v>10</v>
       </c>
-      <c r="G14" s="20" t="n">
+      <c r="G14" s="19" t="n">
         <f aca="false">G$9-G6</f>
         <v>-17</v>
       </c>
-      <c r="H14" s="20" t="n">
+      <c r="H14" s="19" t="n">
         <f aca="false">H$9-H6</f>
         <v>-8</v>
       </c>
-      <c r="I14" s="20" t="n">
+      <c r="I14" s="19" t="n">
         <f aca="false">I$9-I6</f>
         <v>-7</v>
       </c>
     </row>
-    <row r="17" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="24" t="n">
+      <c r="B18" s="23" t="n">
         <f aca="false">H12-F12</f>
         <v>6</v>
       </c>
-      <c r="C18" s="25" t="n">
+      <c r="C18" s="24" t="n">
         <f aca="false">F4</f>
         <v>8</v>
       </c>
-      <c r="D18" s="26" t="n">
+      <c r="D18" s="24" t="n">
         <f aca="false">C18-B18</f>
         <v>2</v>
       </c>
     </row>
-    <row r="19" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="27" t="n">
+      <c r="B19" s="25" t="n">
         <f aca="false">B13-F13</f>
         <v>12</v>
       </c>
-      <c r="C19" s="25" t="n">
+      <c r="C19" s="24" t="n">
         <f aca="false">F5</f>
         <v>22</v>
       </c>
-      <c r="D19" s="27" t="n">
+      <c r="D19" s="25" t="n">
         <f aca="false">C19-B19</f>
         <v>10</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="28"/>
-      <c r="J19" s="30"/>
-    </row>
-    <row r="20" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="s">
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="26"/>
+      <c r="J19" s="28"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="27" t="n">
+      <c r="B20" s="25" t="n">
         <f aca="false">F14-F14</f>
         <v>0</v>
       </c>
-      <c r="C20" s="25" t="n">
+      <c r="C20" s="24" t="n">
         <f aca="false">F6</f>
         <v>0</v>
       </c>
-      <c r="D20" s="26" t="n">
+      <c r="D20" s="24" t="n">
         <f aca="false">C20-B20</f>
         <v>0</v>
       </c>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="26" t="n">
+      <c r="B21" s="24" t="n">
         <f aca="false">-SUM(B18:B20)</f>
         <v>-18</v>
       </c>
-      <c r="C21" s="25" t="n">
+      <c r="C21" s="24" t="n">
         <f aca="false">F7</f>
         <v>-20</v>
       </c>
-      <c r="D21" s="23" t="n">
+      <c r="D21" s="22" t="n">
         <f aca="false">C21-B21</f>
         <v>-2</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2932,7 +3015,7 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2943,9 +3026,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
@@ -3143,7 +3226,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -3152,7 +3235,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="30" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -3161,7 +3244,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="30" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -3206,7 +3289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
         <v>26</v>
       </c>
@@ -3243,31 +3326,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="20" t="n">
+      <c r="B16" s="19" t="n">
         <f aca="false">B$13-B4</f>
         <v>0</v>
       </c>
-      <c r="C16" s="20" t="n">
+      <c r="C16" s="19" t="n">
         <f aca="false">C$13-C4</f>
         <v>-10</v>
       </c>
-      <c r="D16" s="20" t="n">
+      <c r="D16" s="19" t="n">
         <f aca="false">D$13-D4</f>
         <v>7</v>
       </c>
-      <c r="E16" s="20" t="n">
+      <c r="E16" s="19" t="n">
         <f aca="false">E$13-E4</f>
         <v>-9</v>
       </c>
-      <c r="F16" s="20" t="n">
+      <c r="F16" s="19" t="n">
         <f aca="false">F$13-F4</f>
         <v>2</v>
       </c>
-      <c r="G16" s="20" t="n">
+      <c r="G16" s="19" t="n">
         <f aca="false">G$13-G4</f>
         <v>-9</v>
       </c>
@@ -3275,12 +3358,12 @@
         <f aca="false">H$13-H4</f>
         <v>8</v>
       </c>
-      <c r="I16" s="20" t="n">
+      <c r="I16" s="19" t="n">
         <f aca="false">I$13-I4</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -3288,52 +3371,52 @@
         <f aca="false">B$13-B5</f>
         <v>0</v>
       </c>
-      <c r="C17" s="20" t="n">
+      <c r="C17" s="19" t="n">
         <f aca="false">C$13-C5</f>
         <v>-2</v>
       </c>
-      <c r="D17" s="20" t="n">
+      <c r="D17" s="19" t="n">
         <f aca="false">D$13-D5</f>
         <v>-15</v>
       </c>
-      <c r="E17" s="20" t="n">
+      <c r="E17" s="19" t="n">
         <f aca="false">E$13-E5</f>
         <v>-9</v>
       </c>
-      <c r="F17" s="20" t="n">
+      <c r="F17" s="19" t="n">
         <f aca="false">F$13-F5</f>
         <v>-12</v>
       </c>
-      <c r="G17" s="20" t="n">
+      <c r="G17" s="19" t="n">
         <f aca="false">G$13-G5</f>
         <v>-1</v>
       </c>
-      <c r="H17" s="20" t="n">
+      <c r="H17" s="19" t="n">
         <f aca="false">H$13-H5</f>
         <v>-14</v>
       </c>
-      <c r="I17" s="20" t="n">
+      <c r="I17" s="19" t="n">
         <f aca="false">I$13-I5</f>
         <v>-13</v>
       </c>
     </row>
-    <row r="18" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="20" t="n">
+      <c r="B18" s="19" t="n">
         <f aca="false">B$13-B6</f>
         <v>0</v>
       </c>
-      <c r="C18" s="20" t="n">
+      <c r="C18" s="19" t="n">
         <f aca="false">C$13-C6</f>
         <v>-2</v>
       </c>
-      <c r="D18" s="20" t="n">
+      <c r="D18" s="19" t="n">
         <f aca="false">D$13-D6</f>
         <v>7</v>
       </c>
-      <c r="E18" s="20" t="n">
+      <c r="E18" s="19" t="n">
         <f aca="false">E$13-E6</f>
         <v>-25</v>
       </c>
@@ -3341,120 +3424,116 @@
         <f aca="false">F$13-F6</f>
         <v>10</v>
       </c>
-      <c r="G18" s="20" t="n">
+      <c r="G18" s="19" t="n">
         <f aca="false">G$13-G6</f>
         <v>-17</v>
       </c>
-      <c r="H18" s="20" t="n">
+      <c r="H18" s="19" t="n">
         <f aca="false">H$13-H6</f>
         <v>-8</v>
       </c>
-      <c r="I18" s="20" t="n">
+      <c r="I18" s="19" t="n">
         <f aca="false">I$13-I6</f>
         <v>-7</v>
       </c>
     </row>
-    <row r="21" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="24" t="n">
+      <c r="B22" s="23" t="n">
         <f aca="false">H16-F16</f>
         <v>6</v>
       </c>
-      <c r="C22" s="25" t="n">
+      <c r="C22" s="24" t="n">
         <f aca="false">F4</f>
         <v>8</v>
       </c>
-      <c r="D22" s="26" t="n">
+      <c r="D22" s="24" t="n">
         <f aca="false">C22-B22</f>
         <v>2</v>
       </c>
     </row>
-    <row r="23" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="27" t="n">
+      <c r="B23" s="25" t="n">
         <f aca="false">B17-F17</f>
         <v>12</v>
       </c>
-      <c r="C23" s="25" t="n">
+      <c r="C23" s="24" t="n">
         <f aca="false">F5</f>
         <v>22</v>
       </c>
-      <c r="D23" s="27" t="n">
+      <c r="D23" s="25" t="n">
         <f aca="false">C23-B23</f>
         <v>10</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="28"/>
-      <c r="J23" s="30"/>
-    </row>
-    <row r="24" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="26"/>
+      <c r="J23" s="28"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="27" t="n">
+      <c r="B24" s="25" t="n">
         <f aca="false">F18-F18</f>
         <v>0</v>
       </c>
-      <c r="C24" s="25" t="n">
+      <c r="C24" s="24" t="n">
         <f aca="false">F6</f>
         <v>0</v>
       </c>
-      <c r="D24" s="26" t="n">
+      <c r="D24" s="24" t="n">
         <f aca="false">C24-B24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="26" t="n">
+      <c r="B25" s="24" t="n">
         <f aca="false">-SUM(B22:B24)</f>
         <v>-18</v>
       </c>
-      <c r="C25" s="25" t="n">
+      <c r="C25" s="24" t="n">
         <f aca="false">F7</f>
         <v>-20</v>
       </c>
-      <c r="D25" s="23" t="n">
+      <c r="D25" s="22" t="n">
         <f aca="false">C25-B25</f>
         <v>-2</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
-      <c r="B30" s="0"/>
-      <c r="C30" s="0"/>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>